<commit_message>
generate report to upload to archive
</commit_message>
<xml_diff>
--- a/templates/report.xlsx
+++ b/templates/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\GitHub\WRF_Analysis\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C309DE0-AF7B-4333-86A6-37DB16159DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D2F7C6-634D-45E7-9F37-53F1914337BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{58E0C250-4A96-4F50-97B6-68A921CF53CE}"/>
   </bookViews>
@@ -290,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -299,9 +299,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,7 +374,95 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{699D9571-3A4F-4196-B2D9-173F02839BB0}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -829,7 +914,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B6" sqref="B6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -846,11 +931,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -858,8 +943,8 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
       <c r="D2" t="b">
         <f>AND(LEN(SHOT_ID)=15,ISTEXT(LEFT(SHOT_ID,1))=TRUE,MID(SHOT_ID,8,1)="-",ISNUMBER(VALUE(MID(SHOT_ID,2,6))),MID(SHOT_ID,12,1)="-",ISNUMBER(VALUE(MID(SHOT_ID,9,3))),ISNUMBER(VALUE(MID(SHOT_ID,13,3))))</f>
         <v>0</v>
@@ -869,62 +954,62 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="4" t="b">
-        <f>AND(NOT(ISBLANK(B3)),NOT(ISNA(VLOOKUP(Port,Ports,1,FALSE)=Port)))</f>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" t="b">
+        <f>AND(LEN(Port)=9,ISTEXT(LEFT(Port,1))=TRUE,MID(Port,6,1)="-",ISNUMBER(VALUE(MID(Port,3,3))),ISNUMBER(VALUE(MID(Port,7,3))))</f>
         <v>0</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="25"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -953,131 +1038,131 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12" t="s">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="15" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="12" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="12" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="12" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="12" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="12" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1108,131 +1193,131 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12" t="s">
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="15" t="s">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="12" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="12" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="12" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="12" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" s="12" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1263,131 +1348,131 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="9" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="12" t="s">
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="H30" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="13" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="15" t="s">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="12" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" s="12" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" s="12" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" s="12" t="s">
+      <c r="B35" s="16"/>
+      <c r="C35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="12" t="s">
+      <c r="B36" s="16"/>
+      <c r="C36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1418,131 +1503,131 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="9" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="12" t="s">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="12" t="s">
+      <c r="H40" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="13" t="s">
+      <c r="B41" s="13"/>
+      <c r="C41" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="15" t="s">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" s="12" t="s">
+      <c r="B42" s="16"/>
+      <c r="C42" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" s="12" t="s">
+      <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" s="12" t="s">
+      <c r="B44" s="16"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H45" s="12" t="s">
+      <c r="B45" s="16"/>
+      <c r="C45" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H46" s="12" t="s">
+      <c r="B46" s="16"/>
+      <c r="C46" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1573,126 +1658,126 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="9" t="s">
+      <c r="B50" s="9"/>
+      <c r="C50" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="12" t="s">
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H50" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="13" t="s">
+      <c r="B51" s="13"/>
+      <c r="C51" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="15" t="s">
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H51" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" s="12" t="s">
+      <c r="B52" s="16"/>
+      <c r="C52" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H53" s="12" t="s">
+      <c r="B53" s="16"/>
+      <c r="C53" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H53" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="17"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H54" s="12" t="s">
+      <c r="B54" s="16"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H55" s="12" t="s">
+      <c r="B55" s="16"/>
+      <c r="C55" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H55" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H56" s="12" t="s">
+      <c r="B56" s="16"/>
+      <c r="C56" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1706,6 +1791,40 @@
     <mergeCell ref="B5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" stopIfTrue="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D3">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
     <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -1713,7 +1832,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D3">
     <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -1722,21 +1841,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D3">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
-      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>